<commit_message>
add tc search for query without result and update scenario docs
</commit_message>
<xml_diff>
--- a/ScenarioTestDocs-Juan-Web.xlsx
+++ b/ScenarioTestDocs-Juan-Web.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="110">
   <si>
     <t>Created By</t>
   </si>
@@ -385,6 +385,30 @@
   </si>
   <si>
     <t>list on sale appear</t>
+  </si>
+  <si>
+    <t>Test Scenario Final Project Web</t>
+  </si>
+  <si>
+    <t>Verify search with query without result</t>
+  </si>
+  <si>
+    <t>query = -----</t>
+  </si>
+  <si>
+    <t>no result text appear</t>
+  </si>
+  <si>
+    <t>BU_009</t>
+  </si>
+  <si>
+    <t>BU_010</t>
+  </si>
+  <si>
+    <t>BU_011</t>
+  </si>
+  <si>
+    <t>BU_012</t>
   </si>
 </sst>
 </file>
@@ -596,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -634,6 +658,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -648,19 +693,38 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -669,52 +733,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -934,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -956,22 +983,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1024,20 +1051,22 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="21">
+      <c r="F3" s="21"/>
+      <c r="G3" s="26">
         <v>44755</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1090,15 +1119,15 @@
       <c r="AB4" s="3"/>
     </row>
     <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="31" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1136,12 +1165,12 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="19"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G6" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="11">
         <v>0</v>
@@ -1198,29 +1227,29 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="37" t="s">
+      <c r="E8" s="29"/>
+      <c r="F8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="19" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="2"/>
@@ -1244,27 +1273,27 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="34" t="s">
+      <c r="E9" s="35"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="33"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -1286,21 +1315,21 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="31" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33" t="s">
+      <c r="E10" s="35"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="33"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -1322,19 +1351,19 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="31" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="33" t="s">
+      <c r="E11" s="27"/>
+      <c r="F11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1356,21 +1385,21 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="31" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
+      <c r="E12" s="27"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J12" s="2"/>
@@ -1394,25 +1423,25 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="33"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1434,21 +1463,21 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="31" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33" t="s">
+      <c r="E14" s="30"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="33"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -1470,21 +1499,21 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="31" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33" t="s">
+      <c r="E15" s="27"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J15" s="4"/>
@@ -1508,25 +1537,25 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34" t="s">
+      <c r="E16" s="35"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="33"/>
+      <c r="I16" s="17"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1548,21 +1577,21 @@
       <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="31" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33" t="s">
+      <c r="E17" s="35"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="33"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1584,19 +1613,19 @@
       <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="31" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="30" t="s">
+      <c r="E18" s="27"/>
+      <c r="F18" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1618,21 +1647,21 @@
       <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="31" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J19" s="3"/>
@@ -1656,25 +1685,25 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="27" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34" t="s">
+      <c r="E20" s="35"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="33"/>
+      <c r="I20" s="17"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1696,21 +1725,21 @@
       <c r="AB20" s="3"/>
     </row>
     <row r="21" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="31" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33" t="s">
+      <c r="E21" s="35"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="33"/>
+      <c r="I21" s="17"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1732,19 +1761,19 @@
       <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="31" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="30" t="s">
+      <c r="E22" s="27"/>
+      <c r="F22" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1766,21 +1795,21 @@
       <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="31" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="30" t="s">
+      <c r="E23" s="27"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="H23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J23" s="3"/>
@@ -1804,27 +1833,27 @@
       <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="34" t="s">
+      <c r="E24" s="35"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="33"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1846,21 +1875,21 @@
       <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="29" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33" t="s">
+      <c r="E25" s="35"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1882,19 +1911,19 @@
       <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="29" t="s">
+      <c r="A26" s="29"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="30" t="s">
+      <c r="E26" s="27"/>
+      <c r="F26" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1916,21 +1945,21 @@
       <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="29" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="30" t="s">
+      <c r="E27" s="27"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I27" s="33" t="s">
+      <c r="I27" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J27" s="3"/>
@@ -1954,25 +1983,25 @@
       <c r="AB27" s="3"/>
     </row>
     <row r="28" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27" t="s">
+      <c r="B28" s="40"/>
+      <c r="C28" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="34" t="s">
+      <c r="E28" s="27"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="34" t="s">
+      <c r="H28" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="33"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -1994,21 +2023,21 @@
       <c r="AB28" s="3"/>
     </row>
     <row r="29" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="31" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33" t="s">
+      <c r="E29" s="30"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="H29" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I29" s="33"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -2030,21 +2059,21 @@
       <c r="AB29" s="3"/>
     </row>
     <row r="30" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="29" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="30" t="s">
+      <c r="E30" s="27"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="H30" s="30" t="s">
+      <c r="H30" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="33" t="s">
+      <c r="I30" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J30" s="3"/>
@@ -2068,25 +2097,25 @@
       <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="27" t="s">
+      <c r="B31" s="40"/>
+      <c r="C31" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34" t="s">
+      <c r="E31" s="35"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="34" t="s">
+      <c r="H31" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I31" s="33"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -2108,21 +2137,21 @@
       <c r="AB31" s="3"/>
     </row>
     <row r="32" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="31" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33" t="s">
+      <c r="E32" s="35"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="H32" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="33"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -2144,17 +2173,17 @@
       <c r="AB32" s="3"/>
     </row>
     <row r="33" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="29" t="s">
+      <c r="A33" s="34"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -2176,19 +2205,19 @@
       <c r="AB33" s="3"/>
     </row>
     <row r="34" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="24"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="29" t="s">
+      <c r="A34" s="34"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="30" t="s">
+      <c r="E34" s="27"/>
+      <c r="F34" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -2210,21 +2239,21 @@
       <c r="AB34" s="3"/>
     </row>
     <row r="35" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="29" t="s">
+      <c r="A35" s="34"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="30" t="s">
+      <c r="E35" s="27"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="30" t="s">
+      <c r="H35" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="33" t="s">
+      <c r="I35" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J35" s="3"/>
@@ -2248,17 +2277,17 @@
       <c r="AB35" s="3"/>
     </row>
     <row r="36" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="24"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="29" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
@@ -2280,19 +2309,19 @@
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="29" t="s">
+      <c r="A37" s="34"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="30" t="s">
+      <c r="E37" s="27"/>
+      <c r="F37" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -2314,21 +2343,21 @@
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="29" t="s">
+      <c r="A38" s="34"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="30" t="s">
+      <c r="E38" s="27"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H38" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J38" s="3"/>
@@ -2352,27 +2381,27 @@
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="40" t="s">
+      <c r="A39" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="34" t="s">
+      <c r="E39" s="35"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="34" t="s">
+      <c r="H39" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I39" s="33"/>
+      <c r="I39" s="17"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -2395,20 +2424,20 @@
     </row>
     <row r="40" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="41"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="29" t="s">
+      <c r="B40" s="42"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33" t="s">
+      <c r="E40" s="35"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="33" t="s">
+      <c r="H40" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="33"/>
+      <c r="I40" s="17"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -2431,18 +2460,18 @@
     </row>
     <row r="41" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="41"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="29" t="s">
+      <c r="B41" s="42"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="30" t="s">
+      <c r="E41" s="27"/>
+      <c r="F41" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -2465,20 +2494,20 @@
     </row>
     <row r="42" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="41"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="29" t="s">
+      <c r="B42" s="42"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="30" t="s">
+      <c r="E42" s="27"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I42" s="33" t="s">
+      <c r="I42" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J42" s="3"/>
@@ -2502,27 +2531,25 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="31" t="s">
+      <c r="A43" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="42"/>
+      <c r="C43" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="32"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34" t="s">
+      <c r="E43" s="35"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I43" s="33"/>
+      <c r="I43" s="17"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -2544,21 +2571,21 @@
       <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="29" t="s">
+      <c r="A44" s="41"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="32"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33" t="s">
+      <c r="E44" s="35"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="33" t="s">
+      <c r="H44" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="33"/>
+      <c r="I44" s="17"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -2580,17 +2607,19 @@
       <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" s="27"/>
+      <c r="F45" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -2612,21 +2641,23 @@
       <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="H46" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="I46" s="33"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="27"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>6</v>
+      </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -2648,19 +2679,27 @@
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="H47" s="43"/>
-      <c r="I47" s="36"/>
+      <c r="A47" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="35"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="17"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2682,19 +2721,21 @@
       <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E48" s="32"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="H48" s="43"/>
-      <c r="I48" s="36"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="35"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="17"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -2716,19 +2757,17 @@
       <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="H49" s="43"/>
-      <c r="I49" s="36"/>
+      <c r="A49" s="39"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="27"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
@@ -2750,19 +2789,21 @@
       <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="36"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="27"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I50" s="17"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
@@ -2784,17 +2825,19 @@
       <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E51" s="42"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="36"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="35"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H51" s="16"/>
+      <c r="I51" s="14"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -2816,23 +2859,19 @@
       <c r="AB51" s="3"/>
     </row>
     <row r="52" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" s="42"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="H52" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I52" s="33" t="s">
-        <v>6</v>
-      </c>
+      <c r="A52" s="39"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="35"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H52" s="16"/>
+      <c r="I52" s="14"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
@@ -2854,25 +2893,19 @@
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53" s="32"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="I53" s="33"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" s="27"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H53" s="16"/>
+      <c r="I53" s="14"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
@@ -2894,21 +2927,19 @@
       <c r="AB53" s="3"/>
     </row>
     <row r="54" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E54" s="32"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="I54" s="33"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" s="27"/>
+      <c r="F54" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="14"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
@@ -2930,21 +2961,17 @@
       <c r="AB54" s="3"/>
     </row>
     <row r="55" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="25"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E55" s="31"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="H55" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="I55" s="33"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="43"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="14"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
@@ -2966,21 +2993,21 @@
       <c r="AB55" s="3"/>
     </row>
     <row r="56" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="25"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E56" s="31"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="H56" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="I56" s="33" t="s">
+      <c r="A56" s="39"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="43"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I56" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J56" s="3"/>
@@ -3004,25 +3031,25 @@
       <c r="AB56" s="3"/>
     </row>
     <row r="57" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="25"/>
-      <c r="C57" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" s="31" t="s">
+      <c r="A57" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="44"/>
+      <c r="C57" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E57" s="32"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="34" t="s">
+      <c r="E57" s="35"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H57" s="34" t="s">
+      <c r="H57" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I57" s="33"/>
+      <c r="I57" s="17"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
@@ -3044,21 +3071,21 @@
       <c r="AB57" s="3"/>
     </row>
     <row r="58" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="25"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="29" t="s">
+      <c r="A58" s="39"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="32"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33" t="s">
+      <c r="E58" s="35"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H58" s="33" t="s">
+      <c r="H58" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I58" s="33"/>
+      <c r="I58" s="17"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
@@ -3080,21 +3107,21 @@
       <c r="AB58" s="3"/>
     </row>
     <row r="59" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="29" t="s">
+      <c r="A59" s="39"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="E59" s="31"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30" t="s">
+      <c r="E59" s="27"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="H59" s="30" t="s">
+      <c r="H59" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="I59" s="33"/>
+      <c r="I59" s="17"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
@@ -3116,21 +3143,21 @@
       <c r="AB59" s="3"/>
     </row>
     <row r="60" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="25"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="E60" s="31"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="H60" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="I60" s="33" t="s">
+      <c r="A60" s="39"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E60" s="27"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I60" s="17" t="s">
         <v>6</v>
       </c>
       <c r="J60" s="3"/>
@@ -3154,15 +3181,25 @@
       <c r="AB60" s="3"/>
     </row>
     <row r="61" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
+      <c r="A61" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="35"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I61" s="17"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
@@ -3184,15 +3221,21 @@
       <c r="AB61" s="3"/>
     </row>
     <row r="62" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62" s="35"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" s="17"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
@@ -3214,15 +3257,21 @@
       <c r="AB62" s="3"/>
     </row>
     <row r="63" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63" s="27"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I63" s="17"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
@@ -3244,15 +3293,23 @@
       <c r="AB63" s="3"/>
     </row>
     <row r="64" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
+      <c r="A64" s="39"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E64" s="27"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I64" s="17" t="s">
+        <v>6</v>
+      </c>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
@@ -7384,15 +7441,15 @@
       <c r="AB201" s="3"/>
     </row>
     <row r="202" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="2"/>
+      <c r="A202" s="3"/>
       <c r="B202" s="2"/>
-      <c r="C202" s="2"/>
+      <c r="C202" s="3"/>
       <c r="D202" s="3"/>
       <c r="E202" s="3"/>
-      <c r="F202" s="2"/>
-      <c r="G202" s="2"/>
-      <c r="H202" s="2"/>
-      <c r="I202" s="2"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="3"/>
+      <c r="I202" s="3"/>
       <c r="J202" s="2"/>
       <c r="K202" s="2"/>
       <c r="L202" s="2"/>
@@ -7414,15 +7471,15 @@
       <c r="AB202" s="2"/>
     </row>
     <row r="203" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="2"/>
+      <c r="A203" s="3"/>
       <c r="B203" s="2"/>
-      <c r="C203" s="2"/>
-      <c r="D203" s="2"/>
-      <c r="E203" s="2"/>
-      <c r="F203" s="2"/>
-      <c r="G203" s="2"/>
-      <c r="H203" s="2"/>
-      <c r="I203" s="2"/>
+      <c r="C203" s="3"/>
+      <c r="D203" s="3"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="3"/>
+      <c r="G203" s="3"/>
+      <c r="H203" s="3"/>
+      <c r="I203" s="3"/>
       <c r="J203" s="2"/>
       <c r="K203" s="2"/>
       <c r="L203" s="2"/>
@@ -7444,15 +7501,15 @@
       <c r="AB203" s="2"/>
     </row>
     <row r="204" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="2"/>
+      <c r="A204" s="3"/>
       <c r="B204" s="2"/>
-      <c r="C204" s="2"/>
-      <c r="D204" s="2"/>
-      <c r="E204" s="2"/>
-      <c r="F204" s="2"/>
-      <c r="G204" s="2"/>
-      <c r="H204" s="2"/>
-      <c r="I204" s="2"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3"/>
+      <c r="F204" s="3"/>
+      <c r="G204" s="3"/>
+      <c r="H204" s="3"/>
+      <c r="I204" s="3"/>
       <c r="J204" s="2"/>
       <c r="K204" s="2"/>
       <c r="L204" s="2"/>
@@ -7474,15 +7531,15 @@
       <c r="AB204" s="2"/>
     </row>
     <row r="205" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="2"/>
+      <c r="A205" s="3"/>
       <c r="B205" s="2"/>
-      <c r="C205" s="2"/>
-      <c r="D205" s="2"/>
-      <c r="E205" s="2"/>
-      <c r="F205" s="2"/>
-      <c r="G205" s="2"/>
-      <c r="H205" s="2"/>
-      <c r="I205" s="2"/>
+      <c r="C205" s="3"/>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="3"/>
+      <c r="H205" s="3"/>
+      <c r="I205" s="3"/>
       <c r="J205" s="2"/>
       <c r="K205" s="2"/>
       <c r="L205" s="2"/>
@@ -7507,8 +7564,8 @@
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
-      <c r="D206" s="2"/>
-      <c r="E206" s="2"/>
+      <c r="D206" s="3"/>
+      <c r="E206" s="3"/>
       <c r="F206" s="2"/>
       <c r="G206" s="2"/>
       <c r="H206" s="2"/>
@@ -7624,13 +7681,49 @@
       <c r="AB209" s="2"/>
     </row>
     <row r="210" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="2"/>
+      <c r="C210" s="2"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
-    </row>
-    <row r="211" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="F210" s="2"/>
+      <c r="G210" s="2"/>
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+    </row>
+    <row r="211" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
+      <c r="E211" s="2"/>
+      <c r="F211" s="2"/>
+      <c r="G211" s="2"/>
+      <c r="H211" s="2"/>
+      <c r="I211" s="2"/>
+    </row>
+    <row r="212" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
+      <c r="E212" s="2"/>
+      <c r="F212" s="2"/>
+      <c r="G212" s="2"/>
+      <c r="H212" s="2"/>
+      <c r="I212" s="2"/>
+    </row>
+    <row r="213" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="2"/>
+      <c r="C213" s="2"/>
+      <c r="D213" s="2"/>
+      <c r="E213" s="2"/>
+      <c r="F213" s="2"/>
+      <c r="G213" s="2"/>
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+    </row>
+    <row r="214" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D214" s="2"/>
+      <c r="E214" s="2"/>
+    </row>
     <row r="215" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="216" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="217" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8407,41 +8500,45 @@
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="87">
+  <mergeCells count="93">
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="C47:C56"/>
+    <mergeCell ref="A47:A56"/>
     <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B43:B60"/>
     <mergeCell ref="C57:C60"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
-    <mergeCell ref="C43:C52"/>
-    <mergeCell ref="A43:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="C53:C56"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A43:A46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B46"/>
+    <mergeCell ref="B47:B56"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="A31:A38"/>
     <mergeCell ref="B24:B38"/>
     <mergeCell ref="C31:C38"/>
@@ -8456,11 +8553,11 @@
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="C20:C23"/>
@@ -8475,6 +8572,8 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>

</xml_diff>